<commit_message>
present mean, median, sd and coloured graphs
</commit_message>
<xml_diff>
--- a/Part2/results_with_hist.xlsx
+++ b/Part2/results_with_hist.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,32 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Documents\COMP_3008\p2\Comp3008Project2\Part2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{661757D2-A492-47E6-9ADA-18173AD9020B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145FEF9E-4C9B-410C-92A6-E6EA12B5C652}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results_with_hist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">results_with_hist!$A$19:$A$23</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">results_with_hist!$B$19:$B$23</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">results_with_hist!$I$25:$I$26</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">results_with_hist!$J$25:$J$26</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">results_with_hist!$I$25:$I$26</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">results_with_hist!$J$25:$J$26</definedName>
-  </definedNames>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>How much do you like the colours?</t>
-  </si>
-  <si>
-    <t>What is your opinion on the mix of colours and text?Â </t>
   </si>
   <si>
     <t>What is your opinion of using text only passwords?</t>
@@ -83,11 +80,20 @@
   <si>
     <t>sd</t>
   </si>
+  <si>
+    <t>What is your opinion on the mix of colours and text?</t>
+  </si>
+  <si>
+    <t>z-test (is neutral (3) or not)</t>
+  </si>
+  <si>
+    <t>t-test p = (compare text and colour)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -13928,54 +13934,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
@@ -14004,7 +14013,7 @@
         <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2">
         <v>4</v>
@@ -14045,7 +14054,7 @@
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3">
         <v>5</v>
@@ -14086,7 +14095,7 @@
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -14127,7 +14136,7 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -14168,7 +14177,7 @@
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K6">
         <v>4</v>
@@ -14209,7 +14218,7 @@
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7">
         <v>5</v>
@@ -14250,7 +14259,7 @@
         <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8">
         <v>5</v>
@@ -14291,7 +14300,7 @@
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K9">
         <v>4</v>
@@ -14332,7 +14341,7 @@
         <v>5</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K10">
         <v>5</v>
@@ -14373,7 +14382,7 @@
         <v>4</v>
       </c>
       <c r="J11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11">
         <v>4</v>
@@ -14414,7 +14423,7 @@
         <v>5</v>
       </c>
       <c r="J12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12">
         <v>5</v>
@@ -14696,7 +14705,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J25">
         <f>COUNTIF(J2:J12,"=YES")</f>
@@ -14705,7 +14714,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J26">
         <f>COUNTIF(J2:J12,"=NO")</f>
@@ -14714,7 +14723,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29">
         <f>AVERAGE(B2:B12)</f>
@@ -14767,7 +14776,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30">
         <f>MEDIAN(B2:B12)</f>
@@ -14820,7 +14829,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <f>_xlfn.STDEV.S(B2:B12)</f>
@@ -14869,6 +14878,56 @@
       <c r="N31">
         <f t="shared" si="7"/>
         <v>1.0090499582190262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <f>_xlfn.Z.TEST(B2:B12,3)</f>
+        <v>3.6384176352941575E-6</v>
+      </c>
+      <c r="C32">
+        <f>_xlfn.Z.TEST(C2:C12,3)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ref="C32:D32" si="8">_xlfn.Z.TEST(D2:D12,3)</f>
+        <v>7.0065079048010654E-4</v>
+      </c>
+      <c r="G32">
+        <f>_xlfn.Z.TEST(G2:G12,3)</f>
+        <v>0.99892201184818286</v>
+      </c>
+      <c r="H32">
+        <f>_xlfn.Z.TEST(H2:H12,3)</f>
+        <v>0.99999991098448859</v>
+      </c>
+      <c r="I32">
+        <f>_xlfn.Z.TEST(I2:I12,3)</f>
+        <v>9.5044662522332935E-4</v>
+      </c>
+      <c r="K32">
+        <f>_xlfn.Z.TEST(K2:K12,3)</f>
+        <v>1.1377662394818102E-12</v>
+      </c>
+      <c r="N32">
+        <f>_xlfn.Z.TEST(N2:N12,3)</f>
+        <v>0.18501385583113064</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33">
+        <f>_xlfn.T.TEST(E2:E12,F2:F12,2,1)</f>
+        <v>0.43157874584841738</v>
+      </c>
+      <c r="L33">
+        <f>_xlfn.T.TEST(L2:L12,M2:M12,2,1)</f>
+        <v>0.6760811849183086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split box plot into 3
</commit_message>
<xml_diff>
--- a/Part2/results_with_hist.xlsx
+++ b/Part2/results_with_hist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Documents\COMP_3008\p2\Comp3008Project2\Part2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145FEF9E-4C9B-410C-92A6-E6EA12B5C652}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC1026-A7D8-4D96-84D9-E1A905F3EF37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>How much do you like the colours?</t>
   </si>
@@ -82,12 +82,6 @@
   </si>
   <si>
     <t>What is your opinion on the mix of colours and text?</t>
-  </si>
-  <si>
-    <t>z-test (is neutral (3) or not)</t>
-  </si>
-  <si>
-    <t>t-test p = (compare text and colour)</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1123,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="00B050"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -1538,7 +1532,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -1970,7 +1964,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="002060"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -2811,7 +2805,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -3220,7 +3214,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="7030A0"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -3629,7 +3623,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="00B050"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -4061,7 +4055,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="002060"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -4470,7 +4464,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -5288,7 +5282,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -5311,7 +5305,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
@@ -5697,7 +5691,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="7030A0"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -13935,10 +13929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="AD21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BD22" sqref="BD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14174,7 +14168,7 @@
         <v>2</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J6" t="s">
         <v>12</v>
@@ -14578,7 +14572,7 @@
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21">
         <f t="shared" si="2"/>
@@ -14755,7 +14749,7 @@
       </c>
       <c r="I29">
         <f t="shared" si="5"/>
-        <v>3.8181818181818183</v>
+        <v>3.5454545454545454</v>
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
@@ -14861,7 +14855,7 @@
       </c>
       <c r="I31">
         <f t="shared" si="7"/>
-        <v>0.87386289750530233</v>
+        <v>1.4396969378057562</v>
       </c>
       <c r="K31">
         <f t="shared" si="7"/>
@@ -14878,56 +14872,6 @@
       <c r="N31">
         <f t="shared" si="7"/>
         <v>1.0090499582190262</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <f>_xlfn.Z.TEST(B2:B12,3)</f>
-        <v>3.6384176352941575E-6</v>
-      </c>
-      <c r="C32">
-        <f>_xlfn.Z.TEST(C2:C12,3)</f>
-        <v>0.5</v>
-      </c>
-      <c r="D32">
-        <f t="shared" ref="C32:D32" si="8">_xlfn.Z.TEST(D2:D12,3)</f>
-        <v>7.0065079048010654E-4</v>
-      </c>
-      <c r="G32">
-        <f>_xlfn.Z.TEST(G2:G12,3)</f>
-        <v>0.99892201184818286</v>
-      </c>
-      <c r="H32">
-        <f>_xlfn.Z.TEST(H2:H12,3)</f>
-        <v>0.99999991098448859</v>
-      </c>
-      <c r="I32">
-        <f>_xlfn.Z.TEST(I2:I12,3)</f>
-        <v>9.5044662522332935E-4</v>
-      </c>
-      <c r="K32">
-        <f>_xlfn.Z.TEST(K2:K12,3)</f>
-        <v>1.1377662394818102E-12</v>
-      </c>
-      <c r="N32">
-        <f>_xlfn.Z.TEST(N2:N12,3)</f>
-        <v>0.18501385583113064</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33">
-        <f>_xlfn.T.TEST(E2:E12,F2:F12,2,1)</f>
-        <v>0.43157874584841738</v>
-      </c>
-      <c r="L33">
-        <f>_xlfn.T.TEST(L2:L12,M2:M12,2,1)</f>
-        <v>0.6760811849183086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slight changes to excel sheet, to fix minor graph error
</commit_message>
<xml_diff>
--- a/Part2/results_with_hist.xlsx
+++ b/Part2/results_with_hist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Documents\COMP_3008\p2\Comp3008Project2\Part2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\3008-P2\Comp3008Project2\Part2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC1026-A7D8-4D96-84D9-E1A905F3EF37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8881CFF-441D-4FB5-B856-F4FE222F6463}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="789" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results_with_hist" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>How much do you like the colours?</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>What is your opinion on the mix of colours and text?</t>
+  </si>
+  <si>
+    <t>Yes/No's to numeric value</t>
+  </si>
+  <si>
+    <t>Question Number</t>
   </si>
 </sst>
 </file>
@@ -1077,415 +1083,6 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri" panose="020F0502020204030204"/>
               </a:rPr>
-              <a:t>It is easy to learn how to use the colour&amp;text password.</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>results_with_hist!$K$19:$K$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CCD8-4F21-BB3E-A2B23A567849}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="25"/>
-        <c:axId val="556327728"/>
-        <c:axId val="556328056"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="556327728"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-CA"/>
-                  <a:t>Response</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="556328056"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="556328056"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-CA"/>
-                  <a:t>Frequency</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="556327728"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              </a:rPr>
               <a:t>I feel that colour&amp;text passwords are secure.</a:t>
             </a:r>
           </a:p>
@@ -1852,7 +1449,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2284,7 +1881,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2661,6 +2258,302 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="556327728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>I use a Password manager.</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>results_with_hist!$I$25:$I$26</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Yes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>No</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>results_with_hist!$J$25:$J$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8807-4D5B-B0F7-BE4B8878A6ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="741056664"/>
+        <c:axId val="741060272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="741056664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="741060272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="741060272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="741056664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5645,7 +5538,7 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri" panose="020F0502020204030204"/>
               </a:rPr>
-              <a:t>I use a Password manager.</a:t>
+              <a:t>It is easy to learn how to use the colour&amp;text password.</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5691,7 +5584,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="7030A0"/>
+              <a:srgbClr val="00B050"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -5703,7 +5596,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>results_with_hist!$D$19:$D$23</c:f>
+              <c:f>results_with_hist!$K$19:$K$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5711,23 +5604,23 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BB76-446F-96DF-A180954F83E1}"/>
+              <c16:uniqueId val="{00000000-CCD8-4F21-BB3E-A2B23A567849}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8564,7 +8457,7 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8575,7 +8468,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -8598,7 +8491,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -8621,7 +8514,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -8629,11 +8522,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -8658,46 +8551,36 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -8712,8 +8595,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -8721,12 +8606,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -8736,13 +8618,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -8761,16 +8643,18 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -8841,6 +8725,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -8872,8 +8762,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8928,7 +8818,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -8956,18 +8846,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -8977,9 +8856,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -8995,7 +8877,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -9011,7 +8893,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -9025,7 +8907,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -9058,7 +8940,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -9067,6 +8949,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -13441,44 +13329,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Chart 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DE28962-DC56-4E0A-875A-6F6FCAA54D52}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>44</xdr:col>
       <xdr:colOff>163830</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -13509,7 +13359,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13547,7 +13397,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13585,7 +13435,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13616,6 +13466,42 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>7816</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>343877</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>138398</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FED8F24-C3B3-43BE-A813-D4CCE9F0CA1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -13929,10 +13815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="BD22" sqref="BD22"/>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="45" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13940,7 +13826,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -13980,8 +13866,11 @@
       <c r="N1" t="s">
         <v>11</v>
       </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>5</v>
       </c>
@@ -14021,8 +13910,12 @@
       <c r="N2">
         <v>4</v>
       </c>
+      <c r="O2">
+        <f>IF(J2="YES",1,0)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>5</v>
       </c>
@@ -14062,8 +13955,12 @@
       <c r="N3">
         <v>4</v>
       </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="0">IF(J3="YES",1,0)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>4</v>
       </c>
@@ -14103,8 +14000,12 @@
       <c r="N4">
         <v>3</v>
       </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -14144,8 +14045,12 @@
       <c r="N5">
         <v>4</v>
       </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>5</v>
       </c>
@@ -14185,8 +14090,12 @@
       <c r="N6">
         <v>3</v>
       </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>3</v>
       </c>
@@ -14226,8 +14135,12 @@
       <c r="N7">
         <v>5</v>
       </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -14267,8 +14180,12 @@
       <c r="N8">
         <v>3</v>
       </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>4</v>
       </c>
@@ -14308,8 +14225,12 @@
       <c r="N9">
         <v>2</v>
       </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>5</v>
       </c>
@@ -14349,8 +14270,12 @@
       <c r="N10">
         <v>2</v>
       </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>4</v>
       </c>
@@ -14390,8 +14315,12 @@
       <c r="N11">
         <v>2</v>
       </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>3</v>
       </c>
@@ -14430,6 +14359,10 @@
       </c>
       <c r="N12">
         <v>4</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -14441,47 +14374,47 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:N19" si="0">COUNTIF(C2:C12,"=1")</f>
+        <f t="shared" ref="C19:N19" si="1">COUNTIF(C2:C12,"=1")</f>
         <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -14494,47 +14427,47 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:N20" si="1">COUNTIF(C2:C12,"=2")</f>
+        <f t="shared" ref="C20:N20" si="2">COUNTIF(C2:C12,"=2")</f>
         <v>4</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -14547,47 +14480,47 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:N21" si="2">COUNTIF(C2:C12,"=3")</f>
+        <f t="shared" ref="C21:N21" si="3">COUNTIF(C2:C12,"=3")</f>
         <v>3</v>
       </c>
       <c r="D21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="M21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="N21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -14600,47 +14533,47 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:N22" si="3">COUNTIF(C2:C12,"=4")</f>
+        <f t="shared" ref="C22:N22" si="4">COUNTIF(C2:C12,"=4")</f>
         <v>4</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="N22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -14653,47 +14586,47 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:N23" si="4">COUNTIF(C2:C12,"=5")</f>
+        <f t="shared" ref="C23:N23" si="5">COUNTIF(C2:C12,"=5")</f>
         <v>0</v>
       </c>
       <c r="D23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="E23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="K23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="N23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -14715,6 +14648,50 @@
         <v>7</v>
       </c>
     </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28">
+        <v>9</v>
+      </c>
+      <c r="K28">
+        <v>10</v>
+      </c>
+      <c r="L28">
+        <v>11</v>
+      </c>
+      <c r="M28">
+        <v>12</v>
+      </c>
+      <c r="N28">
+        <v>13</v>
+      </c>
+    </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
@@ -14724,47 +14701,51 @@
         <v>4.1818181818181817</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:N29" si="5">AVERAGE(C2:C12)</f>
+        <f t="shared" ref="C29:N29" si="6">AVERAGE(C2:C12)</f>
         <v>3</v>
       </c>
       <c r="D29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.9090909090909092</v>
       </c>
       <c r="E29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2727272727272729</v>
       </c>
       <c r="F29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.5454545454545454</v>
       </c>
       <c r="G29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.2727272727272729</v>
       </c>
       <c r="H29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.8181818181818181</v>
       </c>
       <c r="I29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.5454545454545454</v>
       </c>
+      <c r="J29">
+        <f>AVERAGE($O2:$O12)</f>
+        <v>0.36363636363636365</v>
+      </c>
       <c r="K29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.4545454545454541</v>
       </c>
       <c r="L29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.4545454545454546</v>
       </c>
       <c r="M29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.5454545454545454</v>
       </c>
       <c r="N29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2727272727272729</v>
       </c>
     </row>
@@ -14777,47 +14758,51 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:N30" si="6">MEDIAN(C2:C12)</f>
+        <f t="shared" ref="C30:N30" si="7">MEDIAN(C2:C12)</f>
         <v>3</v>
       </c>
       <c r="D30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="E30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="F30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="G30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
+      <c r="J30">
+        <f>MEDIAN($O2:$O12)</f>
+        <v>0</v>
+      </c>
       <c r="K30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="L30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="M30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="N30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
@@ -14830,47 +14815,51 @@
         <v>0.87386289750530233</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:N31" si="7">_xlfn.STDEV.S(C2:C12)</f>
+        <f t="shared" ref="C31:N31" si="8">_xlfn.STDEV.S(C2:C12)</f>
         <v>0.89442719099991586</v>
       </c>
       <c r="D31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.94387980744853883</v>
       </c>
       <c r="E31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1037127426019049</v>
       </c>
       <c r="F31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.52223296786709272</v>
       </c>
       <c r="G31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.78624539310689634</v>
       </c>
       <c r="H31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.75075719352954806</v>
       </c>
       <c r="I31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4396969378057562</v>
       </c>
+      <c r="J31">
+        <f>_xlfn.STDEV.S($O2:$O12)</f>
+        <v>0.50452497910951299</v>
+      </c>
       <c r="K31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.68755165095232806</v>
       </c>
       <c r="L31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.128152149635532</v>
       </c>
       <c r="M31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2135597524338355</v>
       </c>
       <c r="N31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0090499582190262</v>
       </c>
     </row>

</xml_diff>